<commit_message>
Update Catch the Light Project B.O.M (Units of 100).xlsx
</commit_message>
<xml_diff>
--- a/Test Requirements and Data/Catch the Light Project B.O.M (Units of 100).xlsx
+++ b/Test Requirements and Data/Catch the Light Project B.O.M (Units of 100).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimen\Documents\UMD\ECE 388\Lab Code\Catch_The_Light\Test Requirements and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9A3FDF-6534-4599-BCDB-1EA190303E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8766686-E654-4147-85BB-2132FE935DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91F04D41-92BE-43B5-B9A6-27DC169FA4E9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{91F04D41-92BE-43B5-B9A6-27DC169FA4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -725,25 +725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512452E2-98AF-4164-89CE-6A76B1B77DF4}">
   <dimension ref="H8:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.26171875" customWidth="1"/>
+    <col min="9" max="9" width="15.578125" customWidth="1"/>
+    <col min="10" max="10" width="11.41796875" customWidth="1"/>
+    <col min="11" max="11" width="10.578125" customWidth="1"/>
+    <col min="12" max="12" width="14.68359375" customWidth="1"/>
+    <col min="13" max="13" width="14.26171875" customWidth="1"/>
+    <col min="14" max="14" width="21.41796875" customWidth="1"/>
     <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" customWidth="1"/>
-    <col min="17" max="17" width="112.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.26171875" customWidth="1"/>
+    <col min="17" max="17" width="112.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -758,7 +758,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -771,7 +771,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H10" s="2"/>
       <c r="I10" s="14" t="s">
         <v>64</v>
@@ -786,7 +786,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H11" s="3" t="s">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
       </c>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H12" s="3" t="s">
         <v>10</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H13" s="3" t="s">
         <v>16</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H14" s="3" t="s">
         <v>20</v>
       </c>
@@ -917,7 +917,7 @@
       </c>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
@@ -949,7 +949,7 @@
       </c>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H16" s="3" t="s">
         <v>65</v>
       </c>
@@ -983,7 +983,7 @@
       </c>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H20" s="3" t="s">
         <v>40</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H24" s="3" t="s">
         <v>53</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H25" s="3" t="s">
         <v>57</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1288,7 +1288,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:18" x14ac:dyDescent="0.55000000000000004">
       <c r="H28" s="11" t="s">
         <v>66</v>
       </c>

</xml_diff>